<commit_message>
Regression Module created for each variable
Main changes:
1. Created a module for each variable
2. Deleted space before variable name in excel cell (It was causing an
error).
</commit_message>
<xml_diff>
--- a/Data/RV2_tourism_expenses_domestic.xlsx
+++ b/Data/RV2_tourism_expenses_domestic.xlsx
@@ -29,7 +29,7 @@
     <t>year</t>
   </si>
   <si>
-    <t>      expenses_domestic</t>
+    <t>expenses_domestic</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>